<commit_message>
02. 27. - 19:11
</commit_message>
<xml_diff>
--- a/Logiscool/Időnyilvántartás - Február.xlsx
+++ b/Logiscool/Időnyilvántartás - Február.xlsx
@@ -687,7 +687,7 @@
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.53125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1214,11 +1214,11 @@
         <v>0.708333333333333</v>
       </c>
       <c r="D22" s="9" t="n">
-        <v>0.785243055555556</v>
+        <v>0.784722222222222</v>
       </c>
       <c r="E22" s="10" t="n">
         <f aca="false">D22-C22</f>
-        <v>0.0769097222222222</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
@@ -1296,7 +1296,7 @@
       <c r="J25" s="15"/>
       <c r="K25" s="18" t="n">
         <f aca="false">SUM(E19:E25)</f>
-        <v>0.0769097222222222</v>
+        <v>0.0763888888888889</v>
       </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
@@ -1378,11 +1378,15 @@
       <c r="B29" s="8" t="n">
         <v>45715</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
+      <c r="C29" s="9" t="n">
+        <v>0.6875</v>
+      </c>
+      <c r="D29" s="9" t="n">
+        <v>0.78125</v>
+      </c>
       <c r="E29" s="10" t="n">
         <f aca="false">D29-C29</f>
-        <v>0</v>
+        <v>0.09375</v>
       </c>
       <c r="F29" s="9"/>
       <c r="G29" s="9"/>
@@ -1433,7 +1437,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="12" t="n">
         <f aca="false">SUM(E26:E31)</f>
-        <v>0</v>
+        <v>0.09375</v>
       </c>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
@@ -1518,7 +1522,7 @@
       <c r="D35" s="24"/>
       <c r="E35" s="25" t="n">
         <f aca="false">SUM(E3:E34)</f>
-        <v>0.208854166666667</v>
+        <v>0.302083333333333</v>
       </c>
       <c r="F35" s="26"/>
       <c r="G35" s="26"/>

</xml_diff>